<commit_message>
3.0.4: Implement 'preferAlias' switch to input. It replaces name of field to alis.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectTsAliasSample.xlsx
+++ b/meta/objects/BlancoValueObjectTsAliasSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D4F725-D827-B94C-BD0E-E7B2684D216E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E066F967-5855-434F-8F93-A95318DDCD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20840" yWindow="6420" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="6020" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -1708,8 +1708,8 @@
   </sheetPr>
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2616,6 +2616,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="H46:H47"/>
     <mergeCell ref="I46:I47"/>
     <mergeCell ref="A9:B9"/>
@@ -2632,7 +2633,6 @@
     <mergeCell ref="K46:K47"/>
     <mergeCell ref="G46:G47"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">

</xml_diff>